<commit_message>
added some calculations in Excel and changed some selecteed cells (duh)
</commit_message>
<xml_diff>
--- a/data/extras/SV_Jahresberichte/Jahresergebnisse_20.xlsx
+++ b/data/extras/SV_Jahresberichte/Jahresergebnisse_20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\data\extras\SV_Veroeffentlichungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\WU\WARRA\data\extras\SV_Jahresberichte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E78562-5D19-4F00-97D7-87D654505883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7988459F-ED50-4CB4-9C62-9B880B8EFCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22440" yWindow="-16335" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="375">
   <si>
     <t>Versicherungsträger</t>
   </si>
@@ -2084,6 +2084,9 @@
   </si>
   <si>
     <t>Summe der oberen 3</t>
+  </si>
+  <si>
+    <t>Unterschied VSTR-RK</t>
   </si>
 </sst>
 </file>
@@ -3285,7 +3288,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="703">
+  <cellXfs count="704">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4824,48 +4827,49 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="23" fillId="0" borderId="76" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5211,7 +5215,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -6651,10 +6655,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -6681,20 +6685,20 @@
       <c r="M1" s="196"/>
     </row>
     <row r="2" spans="1:13" s="198" customFormat="1" ht="34.15" customHeight="1">
-      <c r="A2" s="587" t="s">
+      <c r="A2" s="588" t="s">
         <v>284</v>
       </c>
-      <c r="B2" s="587"/>
-      <c r="C2" s="587"/>
-      <c r="D2" s="587"/>
-      <c r="E2" s="587"/>
-      <c r="F2" s="587"/>
-      <c r="G2" s="587"/>
-      <c r="H2" s="587"/>
-      <c r="I2" s="587"/>
-      <c r="J2" s="587"/>
-      <c r="K2" s="587"/>
-      <c r="L2" s="587"/>
+      <c r="B2" s="588"/>
+      <c r="C2" s="588"/>
+      <c r="D2" s="588"/>
+      <c r="E2" s="588"/>
+      <c r="F2" s="588"/>
+      <c r="G2" s="588"/>
+      <c r="H2" s="588"/>
+      <c r="I2" s="588"/>
+      <c r="J2" s="588"/>
+      <c r="K2" s="588"/>
+      <c r="L2" s="588"/>
       <c r="M2" s="197"/>
     </row>
     <row r="3" spans="1:13" s="198" customFormat="1" ht="18.75" hidden="1">
@@ -6728,37 +6732,37 @@
       <c r="M4" s="197"/>
     </row>
     <row r="5" spans="1:13" s="198" customFormat="1" ht="18.75">
-      <c r="A5" s="588" t="s">
+      <c r="A5" s="589" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="588"/>
-      <c r="C5" s="588"/>
-      <c r="D5" s="588"/>
-      <c r="E5" s="588"/>
-      <c r="F5" s="588"/>
-      <c r="G5" s="588"/>
-      <c r="H5" s="588"/>
-      <c r="I5" s="588"/>
-      <c r="J5" s="588"/>
-      <c r="K5" s="588"/>
-      <c r="L5" s="588"/>
+      <c r="B5" s="589"/>
+      <c r="C5" s="589"/>
+      <c r="D5" s="589"/>
+      <c r="E5" s="589"/>
+      <c r="F5" s="589"/>
+      <c r="G5" s="589"/>
+      <c r="H5" s="589"/>
+      <c r="I5" s="589"/>
+      <c r="J5" s="589"/>
+      <c r="K5" s="589"/>
+      <c r="L5" s="589"/>
       <c r="M5" s="197"/>
     </row>
     <row r="6" spans="1:13" s="200" customFormat="1" ht="24.6" customHeight="1">
-      <c r="A6" s="588" t="s">
+      <c r="A6" s="589" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="588"/>
-      <c r="C6" s="588"/>
-      <c r="D6" s="588"/>
-      <c r="E6" s="588"/>
-      <c r="F6" s="588"/>
-      <c r="G6" s="588"/>
-      <c r="H6" s="588"/>
-      <c r="I6" s="588"/>
-      <c r="J6" s="588"/>
-      <c r="K6" s="588"/>
-      <c r="L6" s="588"/>
+      <c r="B6" s="589"/>
+      <c r="C6" s="589"/>
+      <c r="D6" s="589"/>
+      <c r="E6" s="589"/>
+      <c r="F6" s="589"/>
+      <c r="G6" s="589"/>
+      <c r="H6" s="589"/>
+      <c r="I6" s="589"/>
+      <c r="J6" s="589"/>
+      <c r="K6" s="589"/>
+      <c r="L6" s="589"/>
       <c r="M6" s="358"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
@@ -7593,7 +7597,12 @@
       <c r="F33" s="367"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="B35" s="702"/>
+      <c r="B35" s="573"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36" s="203" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="215" t="s">
@@ -7603,6 +7612,10 @@
         <f>SUM(B15:B23)</f>
         <v>7278574</v>
       </c>
+      <c r="C37" s="703">
+        <f>B37-B11</f>
+        <v>120571</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="215" t="s">
@@ -7612,6 +7625,10 @@
         <f>SUM(B24:B25)</f>
         <v>1091751</v>
       </c>
+      <c r="C38" s="703">
+        <f t="shared" ref="C38:C39" si="0">B38-B12</f>
+        <v>5165</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="215" t="s">
@@ -7621,6 +7638,11 @@
         <f>SUM(B26:B27)</f>
         <v>1193401</v>
       </c>
+      <c r="C39" s="703">
+        <f t="shared" si="0"/>
+        <v>28215</v>
+      </c>
+      <c r="D39" s="703"/>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="215" t="s">
@@ -7629,6 +7651,16 @@
       <c r="B40" s="203">
         <f>SUM(B37:B39)</f>
         <v>9563726</v>
+      </c>
+      <c r="C40" s="703">
+        <f>B40-B10</f>
+        <v>153951</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="B48" s="203">
+        <f>B24/(B24+B25)</f>
+        <v>0.19474129174143187</v>
       </c>
     </row>
   </sheetData>
@@ -7674,20 +7706,20 @@
       <c r="M1" s="196"/>
     </row>
     <row r="2" spans="1:13" s="198" customFormat="1" ht="34.15" customHeight="1">
-      <c r="A2" s="587" t="s">
+      <c r="A2" s="588" t="s">
         <v>306</v>
       </c>
-      <c r="B2" s="587"/>
-      <c r="C2" s="587"/>
-      <c r="D2" s="587"/>
-      <c r="E2" s="587"/>
-      <c r="F2" s="587"/>
-      <c r="G2" s="587"/>
-      <c r="H2" s="587"/>
-      <c r="I2" s="587"/>
-      <c r="J2" s="587"/>
-      <c r="K2" s="587"/>
-      <c r="L2" s="587"/>
+      <c r="B2" s="588"/>
+      <c r="C2" s="588"/>
+      <c r="D2" s="588"/>
+      <c r="E2" s="588"/>
+      <c r="F2" s="588"/>
+      <c r="G2" s="588"/>
+      <c r="H2" s="588"/>
+      <c r="I2" s="588"/>
+      <c r="J2" s="588"/>
+      <c r="K2" s="588"/>
+      <c r="L2" s="588"/>
       <c r="M2" s="197"/>
     </row>
     <row r="3" spans="1:13" s="198" customFormat="1" ht="18.75" hidden="1">
@@ -7721,37 +7753,37 @@
       <c r="M4" s="197"/>
     </row>
     <row r="5" spans="1:13" s="198" customFormat="1" ht="18.75">
-      <c r="A5" s="588" t="s">
+      <c r="A5" s="589" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="588"/>
-      <c r="C5" s="588"/>
-      <c r="D5" s="588"/>
-      <c r="E5" s="588"/>
-      <c r="F5" s="588"/>
-      <c r="G5" s="588"/>
-      <c r="H5" s="588"/>
-      <c r="I5" s="588"/>
-      <c r="J5" s="588"/>
-      <c r="K5" s="588"/>
-      <c r="L5" s="588"/>
+      <c r="B5" s="589"/>
+      <c r="C5" s="589"/>
+      <c r="D5" s="589"/>
+      <c r="E5" s="589"/>
+      <c r="F5" s="589"/>
+      <c r="G5" s="589"/>
+      <c r="H5" s="589"/>
+      <c r="I5" s="589"/>
+      <c r="J5" s="589"/>
+      <c r="K5" s="589"/>
+      <c r="L5" s="589"/>
       <c r="M5" s="197"/>
     </row>
     <row r="6" spans="1:13" s="200" customFormat="1" ht="24.6" customHeight="1">
-      <c r="A6" s="588" t="s">
+      <c r="A6" s="589" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="588"/>
-      <c r="C6" s="588"/>
-      <c r="D6" s="588"/>
-      <c r="E6" s="588"/>
-      <c r="F6" s="588"/>
-      <c r="G6" s="588"/>
-      <c r="H6" s="588"/>
-      <c r="I6" s="588"/>
-      <c r="J6" s="588"/>
-      <c r="K6" s="588"/>
-      <c r="L6" s="588"/>
+      <c r="B6" s="589"/>
+      <c r="C6" s="589"/>
+      <c r="D6" s="589"/>
+      <c r="E6" s="589"/>
+      <c r="F6" s="589"/>
+      <c r="G6" s="589"/>
+      <c r="H6" s="589"/>
+      <c r="I6" s="589"/>
+      <c r="J6" s="589"/>
+      <c r="K6" s="589"/>
+      <c r="L6" s="589"/>
       <c r="M6" s="358"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
@@ -8628,20 +8660,20 @@
       <c r="M1" s="196"/>
     </row>
     <row r="2" spans="1:13" s="198" customFormat="1" ht="34.15" customHeight="1">
-      <c r="A2" s="587" t="s">
+      <c r="A2" s="588" t="s">
         <v>307</v>
       </c>
-      <c r="B2" s="587"/>
-      <c r="C2" s="587"/>
-      <c r="D2" s="587"/>
-      <c r="E2" s="587"/>
-      <c r="F2" s="587"/>
-      <c r="G2" s="587"/>
-      <c r="H2" s="587"/>
-      <c r="I2" s="587"/>
-      <c r="J2" s="587"/>
-      <c r="K2" s="587"/>
-      <c r="L2" s="587"/>
+      <c r="B2" s="588"/>
+      <c r="C2" s="588"/>
+      <c r="D2" s="588"/>
+      <c r="E2" s="588"/>
+      <c r="F2" s="588"/>
+      <c r="G2" s="588"/>
+      <c r="H2" s="588"/>
+      <c r="I2" s="588"/>
+      <c r="J2" s="588"/>
+      <c r="K2" s="588"/>
+      <c r="L2" s="588"/>
       <c r="M2" s="197"/>
     </row>
     <row r="3" spans="1:13" s="198" customFormat="1" ht="18.75" hidden="1">
@@ -8675,37 +8707,37 @@
       <c r="M4" s="197"/>
     </row>
     <row r="5" spans="1:13" s="198" customFormat="1" ht="18.75">
-      <c r="A5" s="588" t="s">
+      <c r="A5" s="589" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="588"/>
-      <c r="C5" s="588"/>
-      <c r="D5" s="588"/>
-      <c r="E5" s="588"/>
-      <c r="F5" s="588"/>
-      <c r="G5" s="588"/>
-      <c r="H5" s="588"/>
-      <c r="I5" s="588"/>
-      <c r="J5" s="588"/>
-      <c r="K5" s="588"/>
-      <c r="L5" s="588"/>
+      <c r="B5" s="589"/>
+      <c r="C5" s="589"/>
+      <c r="D5" s="589"/>
+      <c r="E5" s="589"/>
+      <c r="F5" s="589"/>
+      <c r="G5" s="589"/>
+      <c r="H5" s="589"/>
+      <c r="I5" s="589"/>
+      <c r="J5" s="589"/>
+      <c r="K5" s="589"/>
+      <c r="L5" s="589"/>
       <c r="M5" s="197"/>
     </row>
     <row r="6" spans="1:13" s="200" customFormat="1" ht="24.6" customHeight="1">
-      <c r="A6" s="588" t="s">
+      <c r="A6" s="589" t="s">
         <v>282</v>
       </c>
-      <c r="B6" s="588"/>
-      <c r="C6" s="588"/>
-      <c r="D6" s="588"/>
-      <c r="E6" s="588"/>
-      <c r="F6" s="588"/>
-      <c r="G6" s="588"/>
-      <c r="H6" s="588"/>
-      <c r="I6" s="588"/>
-      <c r="J6" s="588"/>
-      <c r="K6" s="588"/>
-      <c r="L6" s="588"/>
+      <c r="B6" s="589"/>
+      <c r="C6" s="589"/>
+      <c r="D6" s="589"/>
+      <c r="E6" s="589"/>
+      <c r="F6" s="589"/>
+      <c r="G6" s="589"/>
+      <c r="H6" s="589"/>
+      <c r="I6" s="589"/>
+      <c r="J6" s="589"/>
+      <c r="K6" s="589"/>
+      <c r="L6" s="589"/>
       <c r="M6" s="358"/>
     </row>
     <row r="7" spans="1:13" ht="15" customHeight="1">
@@ -9635,17 +9667,17 @@
       <c r="J2" s="374"/>
     </row>
     <row r="3" spans="1:10" ht="23.45" customHeight="1">
-      <c r="A3" s="589" t="s">
+      <c r="A3" s="590" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="589"/>
-      <c r="C3" s="589"/>
-      <c r="D3" s="589"/>
-      <c r="E3" s="589"/>
-      <c r="F3" s="589"/>
-      <c r="G3" s="589"/>
-      <c r="H3" s="589"/>
-      <c r="I3" s="589"/>
+      <c r="B3" s="590"/>
+      <c r="C3" s="590"/>
+      <c r="D3" s="590"/>
+      <c r="E3" s="590"/>
+      <c r="F3" s="590"/>
+      <c r="G3" s="590"/>
+      <c r="H3" s="590"/>
+      <c r="I3" s="590"/>
       <c r="J3" s="376"/>
     </row>
     <row r="4" spans="1:10" s="371" customFormat="1" ht="23.25" customHeight="1">
@@ -9658,26 +9690,26 @@
       <c r="J4" s="380"/>
     </row>
     <row r="5" spans="1:10" s="371" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="591" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="592" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="594" t="s">
+      <c r="B5" s="593" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="595" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="595"/>
-      <c r="H5" s="595"/>
-      <c r="I5" s="596"/>
+      <c r="D5" s="596"/>
+      <c r="E5" s="596"/>
+      <c r="F5" s="596"/>
+      <c r="G5" s="596"/>
+      <c r="H5" s="596"/>
+      <c r="I5" s="597"/>
       <c r="J5" s="381"/>
     </row>
     <row r="6" spans="1:10" s="371" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A6" s="591"/>
-      <c r="B6" s="593"/>
+      <c r="A6" s="592"/>
+      <c r="B6" s="594"/>
       <c r="C6" s="382" t="s">
         <v>265</v>
       </c>
@@ -10277,17 +10309,17 @@
       <c r="J2" s="374"/>
     </row>
     <row r="3" spans="1:10" ht="23.45" customHeight="1">
-      <c r="A3" s="589" t="s">
+      <c r="A3" s="590" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="589"/>
-      <c r="C3" s="589"/>
-      <c r="D3" s="589"/>
-      <c r="E3" s="589"/>
-      <c r="F3" s="589"/>
-      <c r="G3" s="589"/>
-      <c r="H3" s="589"/>
-      <c r="I3" s="589"/>
+      <c r="B3" s="590"/>
+      <c r="C3" s="590"/>
+      <c r="D3" s="590"/>
+      <c r="E3" s="590"/>
+      <c r="F3" s="590"/>
+      <c r="G3" s="590"/>
+      <c r="H3" s="590"/>
+      <c r="I3" s="590"/>
       <c r="J3" s="376"/>
     </row>
     <row r="4" spans="1:10" s="371" customFormat="1" ht="23.25" customHeight="1">
@@ -10300,26 +10332,26 @@
       <c r="J4" s="380"/>
     </row>
     <row r="5" spans="1:10" s="371" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="591" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="592" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="594" t="s">
+      <c r="B5" s="593" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="595" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="595"/>
-      <c r="H5" s="595"/>
-      <c r="I5" s="596"/>
+      <c r="D5" s="596"/>
+      <c r="E5" s="596"/>
+      <c r="F5" s="596"/>
+      <c r="G5" s="596"/>
+      <c r="H5" s="596"/>
+      <c r="I5" s="597"/>
       <c r="J5" s="381"/>
     </row>
     <row r="6" spans="1:10" s="371" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A6" s="591"/>
-      <c r="B6" s="593"/>
+      <c r="A6" s="592"/>
+      <c r="B6" s="594"/>
       <c r="C6" s="382" t="s">
         <v>265</v>
       </c>
@@ -10919,17 +10951,17 @@
       <c r="J2" s="374"/>
     </row>
     <row r="3" spans="1:10" ht="23.45" customHeight="1">
-      <c r="A3" s="589" t="s">
+      <c r="A3" s="590" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="589"/>
-      <c r="C3" s="589"/>
-      <c r="D3" s="589"/>
-      <c r="E3" s="589"/>
-      <c r="F3" s="589"/>
-      <c r="G3" s="589"/>
-      <c r="H3" s="589"/>
-      <c r="I3" s="589"/>
+      <c r="B3" s="590"/>
+      <c r="C3" s="590"/>
+      <c r="D3" s="590"/>
+      <c r="E3" s="590"/>
+      <c r="F3" s="590"/>
+      <c r="G3" s="590"/>
+      <c r="H3" s="590"/>
+      <c r="I3" s="590"/>
       <c r="J3" s="376"/>
     </row>
     <row r="4" spans="1:10" s="371" customFormat="1" ht="23.25" customHeight="1">
@@ -10942,26 +10974,26 @@
       <c r="J4" s="380"/>
     </row>
     <row r="5" spans="1:10" s="371" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="590" t="s">
+      <c r="A5" s="591" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="592" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="594" t="s">
+      <c r="B5" s="593" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="595" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="595"/>
-      <c r="H5" s="595"/>
-      <c r="I5" s="596"/>
+      <c r="D5" s="596"/>
+      <c r="E5" s="596"/>
+      <c r="F5" s="596"/>
+      <c r="G5" s="596"/>
+      <c r="H5" s="596"/>
+      <c r="I5" s="597"/>
       <c r="J5" s="381"/>
     </row>
     <row r="6" spans="1:10" s="371" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A6" s="591"/>
-      <c r="B6" s="593"/>
+      <c r="A6" s="592"/>
+      <c r="B6" s="594"/>
       <c r="C6" s="382" t="s">
         <v>265</v>
       </c>
@@ -11564,13 +11596,13 @@
       <c r="F3" s="374"/>
     </row>
     <row r="4" spans="1:6" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="589" t="s">
+      <c r="A4" s="590" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="589"/>
-      <c r="C4" s="589"/>
-      <c r="D4" s="589"/>
-      <c r="E4" s="589"/>
+      <c r="B4" s="590"/>
+      <c r="C4" s="590"/>
+      <c r="D4" s="590"/>
+      <c r="E4" s="590"/>
       <c r="F4" s="376"/>
     </row>
     <row r="5" spans="1:6" s="371" customFormat="1" ht="23.25" customHeight="1">
@@ -11582,25 +11614,25 @@
       <c r="F5" s="380"/>
     </row>
     <row r="6" spans="1:6" s="371" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A6" s="590" t="s">
+      <c r="A6" s="591" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="592" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="597" t="s">
+      <c r="B6" s="593" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="598" t="s">
         <v>271</v>
       </c>
-      <c r="D6" s="594" t="s">
+      <c r="D6" s="595" t="s">
         <v>270</v>
       </c>
-      <c r="E6" s="596"/>
+      <c r="E6" s="597"/>
       <c r="F6" s="381"/>
     </row>
     <row r="7" spans="1:6" s="371" customFormat="1" ht="52.5" customHeight="1">
-      <c r="A7" s="591"/>
-      <c r="B7" s="593"/>
-      <c r="C7" s="593"/>
+      <c r="A7" s="592"/>
+      <c r="B7" s="594"/>
+      <c r="C7" s="594"/>
       <c r="D7" s="420" t="s">
         <v>7</v>
       </c>
@@ -12017,17 +12049,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="598" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="599" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="599"/>
-      <c r="E5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="601"/>
       <c r="F5" s="81" t="s">
         <v>1</v>
       </c>
@@ -12038,11 +12070,11 @@
       <c r="K5" s="82"/>
     </row>
     <row r="6" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="601"/>
-      <c r="D6" s="602"/>
-      <c r="E6" s="603"/>
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="602"/>
+      <c r="D6" s="603"/>
+      <c r="E6" s="604"/>
       <c r="F6" s="81" t="s">
         <v>59</v>
       </c>
@@ -12055,8 +12087,8 @@
       <c r="K6" s="82"/>
     </row>
     <row r="7" spans="1:11" ht="26.25" customHeight="1">
-      <c r="A7" s="609"/>
-      <c r="B7" s="606"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="607"/>
       <c r="C7" s="114" t="s">
         <v>73</v>
       </c>
@@ -12551,13 +12583,13 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="23.25" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="610" t="s">
+      <c r="B5" s="611" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="610" t="s">
+      <c r="C5" s="611" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="46" t="s">
@@ -12572,38 +12604,38 @@
       <c r="K5" s="82"/>
     </row>
     <row r="6" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="605"/>
-      <c r="D6" s="613" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="606"/>
+      <c r="D6" s="614" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="612"/>
-      <c r="F6" s="614" t="s">
+      <c r="E6" s="613"/>
+      <c r="F6" s="615" t="s">
         <v>251</v>
       </c>
-      <c r="G6" s="612"/>
-      <c r="H6" s="611" t="s">
+      <c r="G6" s="613"/>
+      <c r="H6" s="612" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="611"/>
-      <c r="J6" s="611"/>
-      <c r="K6" s="612"/>
+      <c r="I6" s="612"/>
+      <c r="J6" s="612"/>
+      <c r="K6" s="613"/>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1">
-      <c r="A7" s="608"/>
-      <c r="B7" s="605"/>
-      <c r="C7" s="605"/>
-      <c r="D7" s="604" t="s">
+      <c r="A7" s="609"/>
+      <c r="B7" s="606"/>
+      <c r="C7" s="606"/>
+      <c r="D7" s="605" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="604" t="s">
+      <c r="E7" s="605" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="604" t="s">
+      <c r="F7" s="605" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="604" t="s">
+      <c r="G7" s="605" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="81" t="s">
@@ -12616,13 +12648,13 @@
       <c r="K7" s="82"/>
     </row>
     <row r="8" spans="1:11" ht="18" customHeight="1">
-      <c r="A8" s="609"/>
-      <c r="B8" s="606"/>
-      <c r="C8" s="606"/>
-      <c r="D8" s="606"/>
-      <c r="E8" s="606"/>
-      <c r="F8" s="606"/>
-      <c r="G8" s="606"/>
+      <c r="A8" s="610"/>
+      <c r="B8" s="607"/>
+      <c r="C8" s="607"/>
+      <c r="D8" s="607"/>
+      <c r="E8" s="607"/>
+      <c r="F8" s="607"/>
+      <c r="G8" s="607"/>
       <c r="H8" s="98" t="s">
         <v>7</v>
       </c>
@@ -13157,13 +13189,13 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="23.1" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="610" t="s">
+      <c r="B5" s="611" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="617" t="s">
+      <c r="C5" s="618" t="s">
         <v>185</v>
       </c>
       <c r="D5" s="80" t="s">
@@ -13180,51 +13212,51 @@
       <c r="M5" s="82"/>
     </row>
     <row r="6" spans="1:13" ht="23.1" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="618"/>
-      <c r="D6" s="620" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="619"/>
+      <c r="D6" s="621" t="s">
         <v>202</v>
       </c>
-      <c r="E6" s="599"/>
-      <c r="F6" s="620" t="s">
+      <c r="E6" s="600"/>
+      <c r="F6" s="621" t="s">
         <v>203</v>
       </c>
-      <c r="G6" s="621"/>
-      <c r="H6" s="620" t="s">
+      <c r="G6" s="622"/>
+      <c r="H6" s="621" t="s">
         <v>204</v>
       </c>
-      <c r="I6" s="621"/>
-      <c r="J6" s="624" t="s">
+      <c r="I6" s="622"/>
+      <c r="J6" s="625" t="s">
         <v>187</v>
       </c>
-      <c r="K6" s="624"/>
-      <c r="L6" s="624"/>
-      <c r="M6" s="625"/>
+      <c r="K6" s="625"/>
+      <c r="L6" s="625"/>
+      <c r="M6" s="626"/>
     </row>
     <row r="7" spans="1:13" ht="57.75" customHeight="1">
-      <c r="A7" s="608"/>
-      <c r="B7" s="605"/>
-      <c r="C7" s="618"/>
-      <c r="D7" s="601"/>
-      <c r="E7" s="602"/>
-      <c r="F7" s="622"/>
-      <c r="G7" s="623"/>
-      <c r="H7" s="622"/>
-      <c r="I7" s="623"/>
-      <c r="J7" s="613" t="s">
+      <c r="A7" s="609"/>
+      <c r="B7" s="606"/>
+      <c r="C7" s="619"/>
+      <c r="D7" s="602"/>
+      <c r="E7" s="603"/>
+      <c r="F7" s="623"/>
+      <c r="G7" s="624"/>
+      <c r="H7" s="623"/>
+      <c r="I7" s="624"/>
+      <c r="J7" s="614" t="s">
         <v>188</v>
       </c>
-      <c r="K7" s="615"/>
-      <c r="L7" s="616" t="s">
+      <c r="K7" s="616"/>
+      <c r="L7" s="617" t="s">
         <v>189</v>
       </c>
-      <c r="M7" s="615"/>
+      <c r="M7" s="616"/>
     </row>
     <row r="8" spans="1:13" ht="23.1" customHeight="1">
-      <c r="A8" s="609"/>
-      <c r="B8" s="606"/>
-      <c r="C8" s="619"/>
+      <c r="A8" s="610"/>
+      <c r="B8" s="607"/>
+      <c r="C8" s="620"/>
       <c r="D8" s="73" t="s">
         <v>7</v>
       </c>
@@ -14845,10 +14877,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A4" s="607" t="s">
+      <c r="A4" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="610" t="s">
+      <c r="B4" s="611" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="80" t="s">
@@ -14867,54 +14899,54 @@
       <c r="L4" s="82"/>
     </row>
     <row r="5" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A5" s="608"/>
-      <c r="B5" s="605"/>
-      <c r="C5" s="604" t="s">
+      <c r="A5" s="609"/>
+      <c r="B5" s="606"/>
+      <c r="C5" s="605" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="620" t="s">
+      <c r="D5" s="621" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="610" t="s">
+      <c r="E5" s="611" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="610" t="s">
+      <c r="F5" s="611" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="81" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="81"/>
-      <c r="I5" s="610" t="s">
+      <c r="I5" s="611" t="s">
         <v>359</v>
       </c>
-      <c r="J5" s="620" t="s">
+      <c r="J5" s="621" t="s">
         <v>360</v>
       </c>
-      <c r="K5" s="610" t="s">
+      <c r="K5" s="611" t="s">
         <v>368</v>
       </c>
-      <c r="L5" s="621" t="s">
+      <c r="L5" s="622" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
-      <c r="A6" s="609"/>
-      <c r="B6" s="606"/>
-      <c r="C6" s="606"/>
-      <c r="D6" s="601"/>
-      <c r="E6" s="606"/>
-      <c r="F6" s="606"/>
+      <c r="A6" s="610"/>
+      <c r="B6" s="607"/>
+      <c r="C6" s="607"/>
+      <c r="D6" s="602"/>
+      <c r="E6" s="607"/>
+      <c r="F6" s="607"/>
       <c r="G6" s="96" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="163" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="606"/>
-      <c r="J6" s="601"/>
-      <c r="K6" s="606"/>
-      <c r="L6" s="603"/>
+      <c r="I6" s="607"/>
+      <c r="J6" s="602"/>
+      <c r="K6" s="607"/>
+      <c r="L6" s="604"/>
     </row>
     <row r="7" spans="1:12" s="41" customFormat="1" ht="18.95" customHeight="1">
       <c r="A7" s="40">
@@ -15835,56 +15867,56 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="449" customFormat="1" ht="20.45" customHeight="1">
-      <c r="A5" s="628" t="s">
+      <c r="A5" s="629" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="630" t="s">
+      <c r="B5" s="631" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="632" t="s">
+      <c r="C5" s="633" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="632" t="s">
+      <c r="D5" s="633" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="217" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="218"/>
-      <c r="G5" s="632" t="s">
+      <c r="G5" s="633" t="s">
         <v>334</v>
       </c>
       <c r="H5" s="217" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="218"/>
-      <c r="J5" s="632" t="s">
+      <c r="J5" s="633" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="626" t="s">
+      <c r="K5" s="627" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="627"/>
+      <c r="L5" s="628"/>
     </row>
     <row r="6" spans="1:12" s="449" customFormat="1" ht="34.5" customHeight="1">
-      <c r="A6" s="629"/>
-      <c r="B6" s="631"/>
-      <c r="C6" s="631"/>
-      <c r="D6" s="633"/>
+      <c r="A6" s="630"/>
+      <c r="B6" s="632"/>
+      <c r="C6" s="632"/>
+      <c r="D6" s="634"/>
       <c r="E6" s="435" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="450" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="631"/>
+      <c r="G6" s="632"/>
       <c r="H6" s="451" t="s">
         <v>336</v>
       </c>
       <c r="I6" s="452" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="633"/>
+      <c r="J6" s="634"/>
       <c r="K6" s="566" t="s">
         <v>337</v>
       </c>
@@ -17311,56 +17343,56 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="449" customFormat="1" ht="20.45" customHeight="1">
-      <c r="A5" s="628" t="s">
+      <c r="A5" s="629" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="630" t="s">
+      <c r="B5" s="631" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="632" t="s">
+      <c r="C5" s="633" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="632" t="s">
+      <c r="D5" s="633" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="217" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="218"/>
-      <c r="G5" s="632" t="s">
+      <c r="G5" s="633" t="s">
         <v>334</v>
       </c>
       <c r="H5" s="433" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="434"/>
-      <c r="J5" s="632" t="s">
+      <c r="J5" s="633" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="626" t="s">
+      <c r="K5" s="627" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="627"/>
+      <c r="L5" s="628"/>
     </row>
     <row r="6" spans="1:12" s="449" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A6" s="629"/>
-      <c r="B6" s="631"/>
-      <c r="C6" s="631"/>
-      <c r="D6" s="633"/>
+      <c r="A6" s="630"/>
+      <c r="B6" s="632"/>
+      <c r="C6" s="632"/>
+      <c r="D6" s="634"/>
       <c r="E6" s="435" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="450" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="631"/>
+      <c r="G6" s="632"/>
       <c r="H6" s="451" t="s">
         <v>336</v>
       </c>
       <c r="I6" s="452" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="633"/>
+      <c r="J6" s="634"/>
       <c r="K6" s="566" t="s">
         <v>337</v>
       </c>
@@ -19215,56 +19247,56 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="21" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A5" s="635" t="s">
+      <c r="A5" s="636" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
+      <c r="B5" s="605" t="s">
         <v>199</v>
       </c>
-      <c r="C5" s="610" t="s">
+      <c r="C5" s="611" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="610" t="s">
+      <c r="D5" s="611" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="80" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="82"/>
-      <c r="G5" s="610" t="s">
+      <c r="G5" s="611" t="s">
         <v>334</v>
       </c>
-      <c r="H5" s="613" t="s">
+      <c r="H5" s="614" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="615"/>
-      <c r="J5" s="610" t="s">
+      <c r="I5" s="616"/>
+      <c r="J5" s="611" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="613" t="s">
+      <c r="K5" s="614" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="615"/>
+      <c r="L5" s="616"/>
     </row>
     <row r="6" spans="1:12" s="21" customFormat="1" ht="43.5" customHeight="1">
-      <c r="A6" s="636"/>
-      <c r="B6" s="606"/>
-      <c r="C6" s="606"/>
-      <c r="D6" s="634"/>
+      <c r="A6" s="637"/>
+      <c r="B6" s="607"/>
+      <c r="C6" s="607"/>
+      <c r="D6" s="635"/>
       <c r="E6" s="117" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="606"/>
+      <c r="G6" s="607"/>
       <c r="H6" s="105" t="s">
         <v>336</v>
       </c>
       <c r="I6" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="634"/>
+      <c r="J6" s="635"/>
       <c r="K6" s="453" t="s">
         <v>337</v>
       </c>
@@ -19753,16 +19785,16 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="610" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="598" t="s">
+      <c r="B5" s="611" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="599" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="600"/>
+      <c r="D5" s="601"/>
       <c r="E5" s="46" t="s">
         <v>247</v>
       </c>
@@ -19775,34 +19807,34 @@
       <c r="L5" s="82"/>
     </row>
     <row r="6" spans="1:12" ht="42" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="637"/>
-      <c r="D6" s="638"/>
-      <c r="E6" s="620" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="638"/>
+      <c r="D6" s="639"/>
+      <c r="E6" s="621" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="600"/>
-      <c r="G6" s="598" t="s">
+      <c r="F6" s="601"/>
+      <c r="G6" s="599" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="600"/>
-      <c r="I6" s="614" t="s">
+      <c r="H6" s="601"/>
+      <c r="I6" s="615" t="s">
         <v>82</v>
       </c>
-      <c r="J6" s="611"/>
-      <c r="K6" s="611"/>
-      <c r="L6" s="612"/>
+      <c r="J6" s="612"/>
+      <c r="K6" s="612"/>
+      <c r="L6" s="613"/>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1">
-      <c r="A7" s="608"/>
-      <c r="B7" s="605"/>
-      <c r="C7" s="601"/>
-      <c r="D7" s="603"/>
-      <c r="E7" s="601"/>
-      <c r="F7" s="603"/>
-      <c r="G7" s="601"/>
-      <c r="H7" s="603"/>
+      <c r="A7" s="609"/>
+      <c r="B7" s="606"/>
+      <c r="C7" s="602"/>
+      <c r="D7" s="604"/>
+      <c r="E7" s="602"/>
+      <c r="F7" s="604"/>
+      <c r="G7" s="602"/>
+      <c r="H7" s="604"/>
       <c r="I7" s="81" t="s">
         <v>83</v>
       </c>
@@ -19813,8 +19845,8 @@
       <c r="L7" s="82"/>
     </row>
     <row r="8" spans="1:12" ht="21" customHeight="1">
-      <c r="A8" s="609"/>
-      <c r="B8" s="606"/>
+      <c r="A8" s="610"/>
+      <c r="B8" s="607"/>
       <c r="C8" s="114" t="s">
         <v>26</v>
       </c>
@@ -20371,16 +20403,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="27.6" customHeight="1">
-      <c r="A4" s="607" t="s">
+      <c r="A4" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="604" t="s">
+      <c r="B4" s="605" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="610" t="s">
+      <c r="C4" s="611" t="s">
         <v>347</v>
       </c>
-      <c r="D4" s="610" t="s">
+      <c r="D4" s="611" t="s">
         <v>117</v>
       </c>
       <c r="E4" s="81" t="s">
@@ -20389,15 +20421,15 @@
       <c r="F4" s="81"/>
       <c r="G4" s="81"/>
       <c r="H4" s="81"/>
-      <c r="I4" s="610" t="s">
+      <c r="I4" s="611" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="37.15" customHeight="1">
-      <c r="A5" s="609"/>
-      <c r="B5" s="606"/>
-      <c r="C5" s="606"/>
-      <c r="D5" s="606"/>
+      <c r="A5" s="610"/>
+      <c r="B5" s="607"/>
+      <c r="C5" s="607"/>
+      <c r="D5" s="607"/>
       <c r="E5" s="97" t="s">
         <v>119</v>
       </c>
@@ -20410,7 +20442,7 @@
       <c r="H5" s="193" t="s">
         <v>122</v>
       </c>
-      <c r="I5" s="606"/>
+      <c r="I5" s="607"/>
     </row>
     <row r="6" spans="1:9" s="41" customFormat="1" ht="34.9" customHeight="1" thickBot="1">
       <c r="A6" s="57">
@@ -20967,13 +20999,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>129</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -20986,13 +21018,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="639"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="640"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -21005,11 +21037,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="640"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="641"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -21411,13 +21443,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>129</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -21430,13 +21462,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="639"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="640"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -21449,11 +21481,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="640"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="641"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -21855,13 +21887,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>129</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -21874,13 +21906,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -21893,11 +21925,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="609"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -22301,13 +22333,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -22320,13 +22352,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -22339,11 +22371,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="609"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -22747,13 +22779,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -22766,13 +22798,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -22785,11 +22817,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="609"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -23193,13 +23225,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="607" t="s">
+      <c r="A5" s="608" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="604" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="610" t="s">
+      <c r="B5" s="605" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="611" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="81" t="s">
@@ -23212,13 +23244,13 @@
       <c r="I5" s="82"/>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="608"/>
-      <c r="B6" s="605"/>
-      <c r="C6" s="641"/>
-      <c r="D6" s="610" t="s">
+      <c r="A6" s="609"/>
+      <c r="B6" s="606"/>
+      <c r="C6" s="642"/>
+      <c r="D6" s="611" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="610" t="s">
+      <c r="E6" s="611" t="s">
         <v>115</v>
       </c>
       <c r="F6" s="80" t="s">
@@ -23231,11 +23263,11 @@
       <c r="I6" s="82"/>
     </row>
     <row r="7" spans="1:9" ht="57" customHeight="1">
-      <c r="A7" s="609"/>
-      <c r="B7" s="606"/>
-      <c r="C7" s="634"/>
-      <c r="D7" s="634"/>
-      <c r="E7" s="634"/>
+      <c r="A7" s="610"/>
+      <c r="B7" s="607"/>
+      <c r="C7" s="635"/>
+      <c r="D7" s="635"/>
+      <c r="E7" s="635"/>
       <c r="F7" s="117" t="s">
         <v>193</v>
       </c>
@@ -23655,13 +23687,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="22.15" customHeight="1">
-      <c r="A6" s="645" t="s">
+      <c r="A6" s="646" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="632" t="s">
+      <c r="B6" s="633" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="632" t="s">
+      <c r="C6" s="633" t="s">
         <v>223</v>
       </c>
       <c r="D6" s="216" t="s">
@@ -23676,9 +23708,9 @@
       <c r="I6" s="218"/>
     </row>
     <row r="7" spans="1:14" ht="62.45" customHeight="1">
-      <c r="A7" s="646"/>
-      <c r="B7" s="631"/>
-      <c r="C7" s="633"/>
+      <c r="A7" s="647"/>
+      <c r="B7" s="632"/>
+      <c r="C7" s="634"/>
       <c r="D7" s="220" t="s">
         <v>224</v>
       </c>
@@ -23702,7 +23734,7 @@
       <c r="A8" s="204">
         <v>1</v>
       </c>
-      <c r="B8" s="647" t="s">
+      <c r="B8" s="648" t="s">
         <v>225</v>
       </c>
       <c r="C8" s="221" t="s">
@@ -23735,7 +23767,7 @@
       <c r="A9" s="208">
         <v>2</v>
       </c>
-      <c r="B9" s="648"/>
+      <c r="B9" s="649"/>
       <c r="C9" s="224" t="s">
         <v>227</v>
       </c>
@@ -23766,7 +23798,7 @@
       <c r="A10" s="208">
         <v>3</v>
       </c>
-      <c r="B10" s="648"/>
+      <c r="B10" s="649"/>
       <c r="C10" s="227" t="s">
         <v>228</v>
       </c>
@@ -23797,7 +23829,7 @@
       <c r="A11" s="208">
         <v>4</v>
       </c>
-      <c r="B11" s="648"/>
+      <c r="B11" s="649"/>
       <c r="C11" s="227" t="s">
         <v>229</v>
       </c>
@@ -23828,7 +23860,7 @@
       <c r="A12" s="208">
         <v>5</v>
       </c>
-      <c r="B12" s="648"/>
+      <c r="B12" s="649"/>
       <c r="C12" s="227" t="s">
         <v>230</v>
       </c>
@@ -23859,7 +23891,7 @@
       <c r="A13" s="208">
         <v>6</v>
       </c>
-      <c r="B13" s="648"/>
+      <c r="B13" s="649"/>
       <c r="C13" s="224" t="s">
         <v>231</v>
       </c>
@@ -23890,7 +23922,7 @@
       <c r="A14" s="208">
         <v>7</v>
       </c>
-      <c r="B14" s="648"/>
+      <c r="B14" s="649"/>
       <c r="C14" s="227" t="s">
         <v>232</v>
       </c>
@@ -23921,7 +23953,7 @@
       <c r="A15" s="208">
         <v>8</v>
       </c>
-      <c r="B15" s="648"/>
+      <c r="B15" s="649"/>
       <c r="C15" s="227" t="s">
         <v>233</v>
       </c>
@@ -23952,7 +23984,7 @@
       <c r="A16" s="208">
         <v>9</v>
       </c>
-      <c r="B16" s="648"/>
+      <c r="B16" s="649"/>
       <c r="C16" s="224" t="s">
         <v>234</v>
       </c>
@@ -23983,7 +24015,7 @@
       <c r="A17" s="208">
         <v>10</v>
       </c>
-      <c r="B17" s="648"/>
+      <c r="B17" s="649"/>
       <c r="C17" s="227" t="s">
         <v>235</v>
       </c>
@@ -24014,7 +24046,7 @@
       <c r="A18" s="208">
         <v>11</v>
       </c>
-      <c r="B18" s="648"/>
+      <c r="B18" s="649"/>
       <c r="C18" s="227" t="s">
         <v>236</v>
       </c>
@@ -24045,7 +24077,7 @@
       <c r="A19" s="212">
         <v>12</v>
       </c>
-      <c r="B19" s="649"/>
+      <c r="B19" s="650"/>
       <c r="C19" s="228" t="s">
         <v>237</v>
       </c>
@@ -24076,7 +24108,7 @@
       <c r="A20" s="213">
         <v>13</v>
       </c>
-      <c r="B20" s="650" t="s">
+      <c r="B20" s="651" t="s">
         <v>252</v>
       </c>
       <c r="C20" s="231" t="s">
@@ -24109,7 +24141,7 @@
       <c r="A21" s="208">
         <v>14</v>
       </c>
-      <c r="B21" s="643"/>
+      <c r="B21" s="644"/>
       <c r="C21" s="224" t="s">
         <v>238</v>
       </c>
@@ -24140,7 +24172,7 @@
       <c r="A22" s="208">
         <v>15</v>
       </c>
-      <c r="B22" s="643"/>
+      <c r="B22" s="644"/>
       <c r="C22" s="227" t="s">
         <v>228</v>
       </c>
@@ -24171,7 +24203,7 @@
       <c r="A23" s="208">
         <v>16</v>
       </c>
-      <c r="B23" s="643"/>
+      <c r="B23" s="644"/>
       <c r="C23" s="227" t="s">
         <v>229</v>
       </c>
@@ -24202,7 +24234,7 @@
       <c r="A24" s="208">
         <v>17</v>
       </c>
-      <c r="B24" s="643"/>
+      <c r="B24" s="644"/>
       <c r="C24" s="227" t="s">
         <v>230</v>
       </c>
@@ -24233,7 +24265,7 @@
       <c r="A25" s="208">
         <v>18</v>
       </c>
-      <c r="B25" s="643"/>
+      <c r="B25" s="644"/>
       <c r="C25" s="224" t="s">
         <v>231</v>
       </c>
@@ -24264,7 +24296,7 @@
       <c r="A26" s="208">
         <v>19</v>
       </c>
-      <c r="B26" s="643"/>
+      <c r="B26" s="644"/>
       <c r="C26" s="227" t="s">
         <v>232</v>
       </c>
@@ -24295,7 +24327,7 @@
       <c r="A27" s="208">
         <v>20</v>
       </c>
-      <c r="B27" s="643"/>
+      <c r="B27" s="644"/>
       <c r="C27" s="227" t="s">
         <v>233</v>
       </c>
@@ -24326,7 +24358,7 @@
       <c r="A28" s="208">
         <v>21</v>
       </c>
-      <c r="B28" s="643"/>
+      <c r="B28" s="644"/>
       <c r="C28" s="224" t="s">
         <v>234</v>
       </c>
@@ -24357,7 +24389,7 @@
       <c r="A29" s="208">
         <v>22</v>
       </c>
-      <c r="B29" s="643"/>
+      <c r="B29" s="644"/>
       <c r="C29" s="227" t="s">
         <v>235</v>
       </c>
@@ -24388,7 +24420,7 @@
       <c r="A30" s="208">
         <v>23</v>
       </c>
-      <c r="B30" s="643"/>
+      <c r="B30" s="644"/>
       <c r="C30" s="227" t="s">
         <v>236</v>
       </c>
@@ -24419,7 +24451,7 @@
       <c r="A31" s="214">
         <v>24</v>
       </c>
-      <c r="B31" s="644"/>
+      <c r="B31" s="645"/>
       <c r="C31" s="234" t="s">
         <v>237</v>
       </c>
@@ -24450,7 +24482,7 @@
       <c r="A32" s="204">
         <v>25</v>
       </c>
-      <c r="B32" s="642" t="s">
+      <c r="B32" s="643" t="s">
         <v>253</v>
       </c>
       <c r="C32" s="237" t="s">
@@ -24483,7 +24515,7 @@
       <c r="A33" s="208">
         <v>26</v>
       </c>
-      <c r="B33" s="643"/>
+      <c r="B33" s="644"/>
       <c r="C33" s="224" t="s">
         <v>239</v>
       </c>
@@ -24514,7 +24546,7 @@
       <c r="A34" s="208">
         <v>27</v>
       </c>
-      <c r="B34" s="643"/>
+      <c r="B34" s="644"/>
       <c r="C34" s="227" t="s">
         <v>228</v>
       </c>
@@ -24545,7 +24577,7 @@
       <c r="A35" s="208">
         <v>28</v>
       </c>
-      <c r="B35" s="643"/>
+      <c r="B35" s="644"/>
       <c r="C35" s="227" t="s">
         <v>229</v>
       </c>
@@ -24576,7 +24608,7 @@
       <c r="A36" s="208">
         <v>29</v>
       </c>
-      <c r="B36" s="643"/>
+      <c r="B36" s="644"/>
       <c r="C36" s="227" t="s">
         <v>230</v>
       </c>
@@ -24607,7 +24639,7 @@
       <c r="A37" s="208">
         <v>30</v>
       </c>
-      <c r="B37" s="643"/>
+      <c r="B37" s="644"/>
       <c r="C37" s="224" t="s">
         <v>231</v>
       </c>
@@ -24638,7 +24670,7 @@
       <c r="A38" s="208">
         <v>31</v>
       </c>
-      <c r="B38" s="643"/>
+      <c r="B38" s="644"/>
       <c r="C38" s="227" t="s">
         <v>232</v>
       </c>
@@ -24669,7 +24701,7 @@
       <c r="A39" s="208">
         <v>32</v>
       </c>
-      <c r="B39" s="643"/>
+      <c r="B39" s="644"/>
       <c r="C39" s="227" t="s">
         <v>233</v>
       </c>
@@ -24700,7 +24732,7 @@
       <c r="A40" s="208">
         <v>33</v>
       </c>
-      <c r="B40" s="643"/>
+      <c r="B40" s="644"/>
       <c r="C40" s="224" t="s">
         <v>234</v>
       </c>
@@ -24731,7 +24763,7 @@
       <c r="A41" s="208">
         <v>34</v>
       </c>
-      <c r="B41" s="643"/>
+      <c r="B41" s="644"/>
       <c r="C41" s="227" t="s">
         <v>235</v>
       </c>
@@ -24762,7 +24794,7 @@
       <c r="A42" s="208">
         <v>35</v>
       </c>
-      <c r="B42" s="643"/>
+      <c r="B42" s="644"/>
       <c r="C42" s="227" t="s">
         <v>236</v>
       </c>
@@ -24793,7 +24825,7 @@
       <c r="A43" s="214">
         <v>36</v>
       </c>
-      <c r="B43" s="644"/>
+      <c r="B43" s="645"/>
       <c r="C43" s="234" t="s">
         <v>237</v>
       </c>
@@ -24919,13 +24951,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.600000000000001" customHeight="1">
-      <c r="A6" s="645" t="s">
+      <c r="A6" s="646" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="632" t="s">
+      <c r="B6" s="633" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="632" t="s">
+      <c r="C6" s="633" t="s">
         <v>223</v>
       </c>
       <c r="D6" s="216" t="s">
@@ -24940,9 +24972,9 @@
       <c r="I6" s="218"/>
     </row>
     <row r="7" spans="1:14" ht="57.6" customHeight="1">
-      <c r="A7" s="646"/>
-      <c r="B7" s="631"/>
-      <c r="C7" s="633"/>
+      <c r="A7" s="647"/>
+      <c r="B7" s="632"/>
+      <c r="C7" s="634"/>
       <c r="D7" s="220" t="s">
         <v>224</v>
       </c>
@@ -24966,7 +24998,7 @@
       <c r="A8" s="242">
         <v>1</v>
       </c>
-      <c r="B8" s="642" t="s">
+      <c r="B8" s="643" t="s">
         <v>254</v>
       </c>
       <c r="C8" s="252" t="s">
@@ -24999,7 +25031,7 @@
       <c r="A9" s="246">
         <v>2</v>
       </c>
-      <c r="B9" s="651"/>
+      <c r="B9" s="652"/>
       <c r="C9" s="224" t="s">
         <v>240</v>
       </c>
@@ -25030,7 +25062,7 @@
       <c r="A10" s="246">
         <v>3</v>
       </c>
-      <c r="B10" s="651"/>
+      <c r="B10" s="652"/>
       <c r="C10" s="224" t="s">
         <v>228</v>
       </c>
@@ -25061,7 +25093,7 @@
       <c r="A11" s="246">
         <v>4</v>
       </c>
-      <c r="B11" s="651"/>
+      <c r="B11" s="652"/>
       <c r="C11" s="224" t="s">
         <v>229</v>
       </c>
@@ -25092,7 +25124,7 @@
       <c r="A12" s="246">
         <v>5</v>
       </c>
-      <c r="B12" s="651"/>
+      <c r="B12" s="652"/>
       <c r="C12" s="224" t="s">
         <v>230</v>
       </c>
@@ -25123,7 +25155,7 @@
       <c r="A13" s="246">
         <v>6</v>
       </c>
-      <c r="B13" s="651"/>
+      <c r="B13" s="652"/>
       <c r="C13" s="224" t="s">
         <v>231</v>
       </c>
@@ -25154,7 +25186,7 @@
       <c r="A14" s="246">
         <v>7</v>
       </c>
-      <c r="B14" s="651"/>
+      <c r="B14" s="652"/>
       <c r="C14" s="224" t="s">
         <v>232</v>
       </c>
@@ -25185,7 +25217,7 @@
       <c r="A15" s="246">
         <v>8</v>
       </c>
-      <c r="B15" s="651"/>
+      <c r="B15" s="652"/>
       <c r="C15" s="224" t="s">
         <v>233</v>
       </c>
@@ -25216,7 +25248,7 @@
       <c r="A16" s="246">
         <v>9</v>
       </c>
-      <c r="B16" s="651"/>
+      <c r="B16" s="652"/>
       <c r="C16" s="224" t="s">
         <v>234</v>
       </c>
@@ -25247,7 +25279,7 @@
       <c r="A17" s="246">
         <v>10</v>
       </c>
-      <c r="B17" s="651"/>
+      <c r="B17" s="652"/>
       <c r="C17" s="224" t="s">
         <v>235</v>
       </c>
@@ -25278,7 +25310,7 @@
       <c r="A18" s="246">
         <v>11</v>
       </c>
-      <c r="B18" s="651"/>
+      <c r="B18" s="652"/>
       <c r="C18" s="224" t="s">
         <v>236</v>
       </c>
@@ -25309,7 +25341,7 @@
       <c r="A19" s="250">
         <v>12</v>
       </c>
-      <c r="B19" s="652"/>
+      <c r="B19" s="653"/>
       <c r="C19" s="255" t="s">
         <v>237</v>
       </c>
@@ -25340,7 +25372,7 @@
       <c r="A20" s="242">
         <v>13</v>
       </c>
-      <c r="B20" s="642" t="s">
+      <c r="B20" s="643" t="s">
         <v>255</v>
       </c>
       <c r="C20" s="252" t="s">
@@ -25373,7 +25405,7 @@
       <c r="A21" s="246">
         <v>14</v>
       </c>
-      <c r="B21" s="651"/>
+      <c r="B21" s="652"/>
       <c r="C21" s="224" t="s">
         <v>241</v>
       </c>
@@ -25404,7 +25436,7 @@
       <c r="A22" s="246">
         <v>15</v>
       </c>
-      <c r="B22" s="651"/>
+      <c r="B22" s="652"/>
       <c r="C22" s="224" t="s">
         <v>228</v>
       </c>
@@ -25435,7 +25467,7 @@
       <c r="A23" s="246">
         <v>16</v>
       </c>
-      <c r="B23" s="651"/>
+      <c r="B23" s="652"/>
       <c r="C23" s="224" t="s">
         <v>229</v>
       </c>
@@ -25466,7 +25498,7 @@
       <c r="A24" s="246">
         <v>17</v>
       </c>
-      <c r="B24" s="651"/>
+      <c r="B24" s="652"/>
       <c r="C24" s="224" t="s">
         <v>230</v>
       </c>
@@ -25497,7 +25529,7 @@
       <c r="A25" s="246">
         <v>18</v>
       </c>
-      <c r="B25" s="651"/>
+      <c r="B25" s="652"/>
       <c r="C25" s="224" t="s">
         <v>231</v>
       </c>
@@ -25528,7 +25560,7 @@
       <c r="A26" s="246">
         <v>19</v>
       </c>
-      <c r="B26" s="651"/>
+      <c r="B26" s="652"/>
       <c r="C26" s="224" t="s">
         <v>232</v>
       </c>
@@ -25559,7 +25591,7 @@
       <c r="A27" s="246">
         <v>20</v>
       </c>
-      <c r="B27" s="651"/>
+      <c r="B27" s="652"/>
       <c r="C27" s="224" t="s">
         <v>233</v>
       </c>
@@ -25590,7 +25622,7 @@
       <c r="A28" s="246">
         <v>21</v>
       </c>
-      <c r="B28" s="651"/>
+      <c r="B28" s="652"/>
       <c r="C28" s="224" t="s">
         <v>234</v>
       </c>
@@ -25621,7 +25653,7 @@
       <c r="A29" s="246">
         <v>22</v>
       </c>
-      <c r="B29" s="651"/>
+      <c r="B29" s="652"/>
       <c r="C29" s="224" t="s">
         <v>235</v>
       </c>
@@ -25652,7 +25684,7 @@
       <c r="A30" s="246">
         <v>23</v>
       </c>
-      <c r="B30" s="651"/>
+      <c r="B30" s="652"/>
       <c r="C30" s="224" t="s">
         <v>236</v>
       </c>
@@ -25683,7 +25715,7 @@
       <c r="A31" s="250">
         <v>24</v>
       </c>
-      <c r="B31" s="652"/>
+      <c r="B31" s="653"/>
       <c r="C31" s="255" t="s">
         <v>237</v>
       </c>
@@ -25714,7 +25746,7 @@
       <c r="A32" s="251">
         <v>25</v>
       </c>
-      <c r="B32" s="642" t="s">
+      <c r="B32" s="643" t="s">
         <v>351</v>
       </c>
       <c r="C32" s="256" t="s">
@@ -25747,7 +25779,7 @@
       <c r="A33" s="246">
         <v>26</v>
       </c>
-      <c r="B33" s="651"/>
+      <c r="B33" s="652"/>
       <c r="C33" s="224" t="s">
         <v>242</v>
       </c>
@@ -25778,7 +25810,7 @@
       <c r="A34" s="246">
         <v>27</v>
       </c>
-      <c r="B34" s="651"/>
+      <c r="B34" s="652"/>
       <c r="C34" s="224" t="s">
         <v>228</v>
       </c>
@@ -25809,7 +25841,7 @@
       <c r="A35" s="246">
         <v>28</v>
       </c>
-      <c r="B35" s="651"/>
+      <c r="B35" s="652"/>
       <c r="C35" s="224" t="s">
         <v>229</v>
       </c>
@@ -25840,7 +25872,7 @@
       <c r="A36" s="246">
         <v>29</v>
       </c>
-      <c r="B36" s="651"/>
+      <c r="B36" s="652"/>
       <c r="C36" s="224" t="s">
         <v>230</v>
       </c>
@@ -25871,7 +25903,7 @@
       <c r="A37" s="246">
         <v>30</v>
       </c>
-      <c r="B37" s="651"/>
+      <c r="B37" s="652"/>
       <c r="C37" s="224" t="s">
         <v>231</v>
       </c>
@@ -25902,7 +25934,7 @@
       <c r="A38" s="246">
         <v>31</v>
       </c>
-      <c r="B38" s="651"/>
+      <c r="B38" s="652"/>
       <c r="C38" s="224" t="s">
         <v>232</v>
       </c>
@@ -25933,7 +25965,7 @@
       <c r="A39" s="246">
         <v>32</v>
       </c>
-      <c r="B39" s="651"/>
+      <c r="B39" s="652"/>
       <c r="C39" s="224" t="s">
         <v>233</v>
       </c>
@@ -25964,7 +25996,7 @@
       <c r="A40" s="246">
         <v>33</v>
       </c>
-      <c r="B40" s="651"/>
+      <c r="B40" s="652"/>
       <c r="C40" s="224" t="s">
         <v>234</v>
       </c>
@@ -25995,7 +26027,7 @@
       <c r="A41" s="246">
         <v>34</v>
       </c>
-      <c r="B41" s="651"/>
+      <c r="B41" s="652"/>
       <c r="C41" s="224" t="s">
         <v>235</v>
       </c>
@@ -26026,7 +26058,7 @@
       <c r="A42" s="246">
         <v>35</v>
       </c>
-      <c r="B42" s="651"/>
+      <c r="B42" s="652"/>
       <c r="C42" s="224" t="s">
         <v>236</v>
       </c>
@@ -26057,7 +26089,7 @@
       <c r="A43" s="250">
         <v>36</v>
       </c>
-      <c r="B43" s="652"/>
+      <c r="B43" s="653"/>
       <c r="C43" s="255" t="s">
         <v>237</v>
       </c>
@@ -26088,7 +26120,7 @@
       <c r="A44" s="242">
         <v>37</v>
       </c>
-      <c r="B44" s="642" t="s">
+      <c r="B44" s="643" t="s">
         <v>352</v>
       </c>
       <c r="C44" s="252" t="s">
@@ -26121,7 +26153,7 @@
       <c r="A45" s="246">
         <v>38</v>
       </c>
-      <c r="B45" s="651"/>
+      <c r="B45" s="652"/>
       <c r="C45" s="224" t="s">
         <v>238</v>
       </c>
@@ -26152,7 +26184,7 @@
       <c r="A46" s="246">
         <v>39</v>
       </c>
-      <c r="B46" s="651"/>
+      <c r="B46" s="652"/>
       <c r="C46" s="224" t="s">
         <v>228</v>
       </c>
@@ -26183,7 +26215,7 @@
       <c r="A47" s="246">
         <v>40</v>
       </c>
-      <c r="B47" s="651"/>
+      <c r="B47" s="652"/>
       <c r="C47" s="224" t="s">
         <v>229</v>
       </c>
@@ -26214,7 +26246,7 @@
       <c r="A48" s="246">
         <v>41</v>
       </c>
-      <c r="B48" s="651"/>
+      <c r="B48" s="652"/>
       <c r="C48" s="224" t="s">
         <v>230</v>
       </c>
@@ -26245,7 +26277,7 @@
       <c r="A49" s="246">
         <v>42</v>
       </c>
-      <c r="B49" s="651"/>
+      <c r="B49" s="652"/>
       <c r="C49" s="224" t="s">
         <v>231</v>
       </c>
@@ -26276,7 +26308,7 @@
       <c r="A50" s="246">
         <v>43</v>
       </c>
-      <c r="B50" s="651"/>
+      <c r="B50" s="652"/>
       <c r="C50" s="224" t="s">
         <v>232</v>
       </c>
@@ -26307,7 +26339,7 @@
       <c r="A51" s="246">
         <v>44</v>
       </c>
-      <c r="B51" s="651"/>
+      <c r="B51" s="652"/>
       <c r="C51" s="224" t="s">
         <v>233</v>
       </c>
@@ -26338,7 +26370,7 @@
       <c r="A52" s="246">
         <v>45</v>
       </c>
-      <c r="B52" s="651"/>
+      <c r="B52" s="652"/>
       <c r="C52" s="224" t="s">
         <v>234</v>
       </c>
@@ -26369,7 +26401,7 @@
       <c r="A53" s="246">
         <v>46</v>
       </c>
-      <c r="B53" s="651"/>
+      <c r="B53" s="652"/>
       <c r="C53" s="224" t="s">
         <v>235</v>
       </c>
@@ -26400,7 +26432,7 @@
       <c r="A54" s="246">
         <v>47</v>
       </c>
-      <c r="B54" s="651"/>
+      <c r="B54" s="652"/>
       <c r="C54" s="224" t="s">
         <v>236</v>
       </c>
@@ -26431,7 +26463,7 @@
       <c r="A55" s="250">
         <v>48</v>
       </c>
-      <c r="B55" s="652"/>
+      <c r="B55" s="653"/>
       <c r="C55" s="255" t="s">
         <v>237</v>
       </c>
@@ -26558,13 +26590,13 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="22.15" customHeight="1">
-      <c r="A6" s="645" t="s">
+      <c r="A6" s="646" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="632" t="s">
+      <c r="B6" s="633" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="632" t="s">
+      <c r="C6" s="633" t="s">
         <v>223</v>
       </c>
       <c r="D6" s="216" t="s">
@@ -26579,9 +26611,9 @@
       <c r="I6" s="218"/>
     </row>
     <row r="7" spans="1:14" ht="62.45" customHeight="1">
-      <c r="A7" s="646"/>
-      <c r="B7" s="631"/>
-      <c r="C7" s="633"/>
+      <c r="A7" s="647"/>
+      <c r="B7" s="632"/>
+      <c r="C7" s="634"/>
       <c r="D7" s="220" t="s">
         <v>224</v>
       </c>
@@ -26605,7 +26637,7 @@
       <c r="A8" s="204">
         <v>1</v>
       </c>
-      <c r="B8" s="642" t="s">
+      <c r="B8" s="643" t="s">
         <v>353</v>
       </c>
       <c r="C8" s="221" t="s">
@@ -26638,7 +26670,7 @@
       <c r="A9" s="208">
         <v>2</v>
       </c>
-      <c r="B9" s="643"/>
+      <c r="B9" s="644"/>
       <c r="C9" s="224" t="s">
         <v>243</v>
       </c>
@@ -26669,7 +26701,7 @@
       <c r="A10" s="208">
         <v>3</v>
       </c>
-      <c r="B10" s="643"/>
+      <c r="B10" s="644"/>
       <c r="C10" s="227" t="s">
         <v>228</v>
       </c>
@@ -26700,7 +26732,7 @@
       <c r="A11" s="208">
         <v>4</v>
       </c>
-      <c r="B11" s="643"/>
+      <c r="B11" s="644"/>
       <c r="C11" s="224" t="s">
         <v>229</v>
       </c>
@@ -26731,7 +26763,7 @@
       <c r="A12" s="208">
         <v>5</v>
       </c>
-      <c r="B12" s="643"/>
+      <c r="B12" s="644"/>
       <c r="C12" s="224" t="s">
         <v>230</v>
       </c>
@@ -26762,7 +26794,7 @@
       <c r="A13" s="208">
         <v>6</v>
       </c>
-      <c r="B13" s="643"/>
+      <c r="B13" s="644"/>
       <c r="C13" s="224" t="s">
         <v>231</v>
       </c>
@@ -26793,7 +26825,7 @@
       <c r="A14" s="208">
         <v>7</v>
       </c>
-      <c r="B14" s="643"/>
+      <c r="B14" s="644"/>
       <c r="C14" s="224" t="s">
         <v>232</v>
       </c>
@@ -26824,7 +26856,7 @@
       <c r="A15" s="208">
         <v>8</v>
       </c>
-      <c r="B15" s="643"/>
+      <c r="B15" s="644"/>
       <c r="C15" s="224" t="s">
         <v>233</v>
       </c>
@@ -26855,7 +26887,7 @@
       <c r="A16" s="208">
         <v>9</v>
       </c>
-      <c r="B16" s="643"/>
+      <c r="B16" s="644"/>
       <c r="C16" s="224" t="s">
         <v>234</v>
       </c>
@@ -26886,7 +26918,7 @@
       <c r="A17" s="208">
         <v>10</v>
       </c>
-      <c r="B17" s="643"/>
+      <c r="B17" s="644"/>
       <c r="C17" s="227" t="s">
         <v>235</v>
       </c>
@@ -26917,7 +26949,7 @@
       <c r="A18" s="208">
         <v>11</v>
       </c>
-      <c r="B18" s="643"/>
+      <c r="B18" s="644"/>
       <c r="C18" s="227" t="s">
         <v>236</v>
       </c>
@@ -26948,7 +26980,7 @@
       <c r="A19" s="214">
         <v>12</v>
       </c>
-      <c r="B19" s="644"/>
+      <c r="B19" s="645"/>
       <c r="C19" s="257" t="s">
         <v>237</v>
       </c>
@@ -26979,7 +27011,7 @@
       <c r="A20" s="204">
         <v>13</v>
       </c>
-      <c r="B20" s="642" t="s">
+      <c r="B20" s="643" t="s">
         <v>354</v>
       </c>
       <c r="C20" s="221" t="s">
@@ -27012,7 +27044,7 @@
       <c r="A21" s="208">
         <v>14</v>
       </c>
-      <c r="B21" s="643"/>
+      <c r="B21" s="644"/>
       <c r="C21" s="224" t="s">
         <v>243</v>
       </c>
@@ -27043,7 +27075,7 @@
       <c r="A22" s="208">
         <v>15</v>
       </c>
-      <c r="B22" s="643"/>
+      <c r="B22" s="644"/>
       <c r="C22" s="227" t="s">
         <v>228</v>
       </c>
@@ -27074,7 +27106,7 @@
       <c r="A23" s="208">
         <v>16</v>
       </c>
-      <c r="B23" s="643"/>
+      <c r="B23" s="644"/>
       <c r="C23" s="224" t="s">
         <v>229</v>
       </c>
@@ -27105,7 +27137,7 @@
       <c r="A24" s="208">
         <v>17</v>
       </c>
-      <c r="B24" s="643"/>
+      <c r="B24" s="644"/>
       <c r="C24" s="224" t="s">
         <v>230</v>
       </c>
@@ -27136,7 +27168,7 @@
       <c r="A25" s="208">
         <v>18</v>
       </c>
-      <c r="B25" s="643"/>
+      <c r="B25" s="644"/>
       <c r="C25" s="224" t="s">
         <v>231</v>
       </c>
@@ -27167,7 +27199,7 @@
       <c r="A26" s="208">
         <v>19</v>
       </c>
-      <c r="B26" s="643"/>
+      <c r="B26" s="644"/>
       <c r="C26" s="224" t="s">
         <v>232</v>
       </c>
@@ -27198,7 +27230,7 @@
       <c r="A27" s="208">
         <v>20</v>
       </c>
-      <c r="B27" s="643"/>
+      <c r="B27" s="644"/>
       <c r="C27" s="224" t="s">
         <v>233</v>
       </c>
@@ -27229,7 +27261,7 @@
       <c r="A28" s="208">
         <v>21</v>
       </c>
-      <c r="B28" s="643"/>
+      <c r="B28" s="644"/>
       <c r="C28" s="224" t="s">
         <v>234</v>
       </c>
@@ -27260,7 +27292,7 @@
       <c r="A29" s="208">
         <v>22</v>
       </c>
-      <c r="B29" s="643"/>
+      <c r="B29" s="644"/>
       <c r="C29" s="227" t="s">
         <v>235</v>
       </c>
@@ -27291,7 +27323,7 @@
       <c r="A30" s="208">
         <v>23</v>
       </c>
-      <c r="B30" s="643"/>
+      <c r="B30" s="644"/>
       <c r="C30" s="227" t="s">
         <v>236</v>
       </c>
@@ -27322,7 +27354,7 @@
       <c r="A31" s="214">
         <v>24</v>
       </c>
-      <c r="B31" s="644"/>
+      <c r="B31" s="645"/>
       <c r="C31" s="257" t="s">
         <v>237</v>
       </c>
@@ -27513,10 +27545,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1">
-      <c r="A5" s="653" t="s">
+      <c r="A5" s="654" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="655" t="s">
+      <c r="B5" s="656" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="258" t="s">
@@ -27527,8 +27559,8 @@
       <c r="F5" s="260"/>
     </row>
     <row r="6" spans="1:6" ht="39" customHeight="1">
-      <c r="A6" s="654"/>
-      <c r="B6" s="574"/>
+      <c r="A6" s="655"/>
+      <c r="B6" s="577"/>
       <c r="C6" s="124" t="s">
         <v>40</v>
       </c>
@@ -29086,13 +29118,13 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="21" customHeight="1">
-      <c r="A5" s="645" t="s">
+      <c r="A5" s="646" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="632" t="s">
+      <c r="B5" s="633" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="632" t="s">
+      <c r="C5" s="633" t="s">
         <v>151</v>
       </c>
       <c r="D5" s="216" t="s">
@@ -29107,9 +29139,9 @@
       <c r="I5" s="218"/>
     </row>
     <row r="6" spans="1:14" ht="21" customHeight="1">
-      <c r="A6" s="659"/>
-      <c r="B6" s="660"/>
-      <c r="C6" s="660"/>
+      <c r="A6" s="660"/>
+      <c r="B6" s="661"/>
+      <c r="C6" s="661"/>
       <c r="D6" s="216" t="s">
         <v>50</v>
       </c>
@@ -29122,9 +29154,9 @@
       <c r="I6" s="434"/>
     </row>
     <row r="7" spans="1:14" ht="21" customHeight="1">
-      <c r="A7" s="646"/>
-      <c r="B7" s="633"/>
-      <c r="C7" s="633"/>
+      <c r="A7" s="647"/>
+      <c r="B7" s="634"/>
+      <c r="C7" s="634"/>
       <c r="D7" s="435">
         <v>2020</v>
       </c>
@@ -29148,7 +29180,7 @@
       <c r="A8" s="437">
         <v>1</v>
       </c>
-      <c r="B8" s="656" t="s">
+      <c r="B8" s="657" t="s">
         <v>153</v>
       </c>
       <c r="C8" s="237" t="s">
@@ -29181,7 +29213,7 @@
       <c r="A9" s="208">
         <v>2</v>
       </c>
-      <c r="B9" s="661"/>
+      <c r="B9" s="662"/>
       <c r="C9" s="224" t="s">
         <v>154</v>
       </c>
@@ -29212,7 +29244,7 @@
       <c r="A10" s="208">
         <v>3</v>
       </c>
-      <c r="B10" s="661"/>
+      <c r="B10" s="662"/>
       <c r="C10" s="227" t="s">
         <v>155</v>
       </c>
@@ -29243,7 +29275,7 @@
       <c r="A11" s="208">
         <v>4</v>
       </c>
-      <c r="B11" s="661"/>
+      <c r="B11" s="662"/>
       <c r="C11" s="227" t="s">
         <v>156</v>
       </c>
@@ -29274,7 +29306,7 @@
       <c r="A12" s="208">
         <v>5</v>
       </c>
-      <c r="B12" s="661"/>
+      <c r="B12" s="662"/>
       <c r="C12" s="227" t="s">
         <v>157</v>
       </c>
@@ -29305,7 +29337,7 @@
       <c r="A13" s="208">
         <v>6</v>
       </c>
-      <c r="B13" s="661"/>
+      <c r="B13" s="662"/>
       <c r="C13" s="227" t="s">
         <v>158</v>
       </c>
@@ -29336,7 +29368,7 @@
       <c r="A14" s="208">
         <v>7</v>
       </c>
-      <c r="B14" s="661"/>
+      <c r="B14" s="662"/>
       <c r="C14" s="227" t="s">
         <v>159</v>
       </c>
@@ -29367,7 +29399,7 @@
       <c r="A15" s="208">
         <v>8</v>
       </c>
-      <c r="B15" s="661"/>
+      <c r="B15" s="662"/>
       <c r="C15" s="227" t="s">
         <v>160</v>
       </c>
@@ -29398,7 +29430,7 @@
       <c r="A16" s="208">
         <v>9</v>
       </c>
-      <c r="B16" s="661"/>
+      <c r="B16" s="662"/>
       <c r="C16" s="227" t="s">
         <v>161</v>
       </c>
@@ -29429,7 +29461,7 @@
       <c r="A17" s="214">
         <v>10</v>
       </c>
-      <c r="B17" s="662"/>
+      <c r="B17" s="663"/>
       <c r="C17" s="257" t="s">
         <v>162</v>
       </c>
@@ -29460,7 +29492,7 @@
       <c r="A18" s="437">
         <v>11</v>
       </c>
-      <c r="B18" s="656" t="s">
+      <c r="B18" s="657" t="s">
         <v>163</v>
       </c>
       <c r="C18" s="237" t="s">
@@ -29493,7 +29525,7 @@
       <c r="A19" s="208">
         <v>12</v>
       </c>
-      <c r="B19" s="661"/>
+      <c r="B19" s="662"/>
       <c r="C19" s="224" t="s">
         <v>154</v>
       </c>
@@ -29524,7 +29556,7 @@
       <c r="A20" s="208">
         <v>13</v>
       </c>
-      <c r="B20" s="661"/>
+      <c r="B20" s="662"/>
       <c r="C20" s="227" t="s">
         <v>155</v>
       </c>
@@ -29555,7 +29587,7 @@
       <c r="A21" s="208">
         <v>14</v>
       </c>
-      <c r="B21" s="661"/>
+      <c r="B21" s="662"/>
       <c r="C21" s="227" t="s">
         <v>156</v>
       </c>
@@ -29586,7 +29618,7 @@
       <c r="A22" s="208">
         <v>15</v>
       </c>
-      <c r="B22" s="661"/>
+      <c r="B22" s="662"/>
       <c r="C22" s="227" t="s">
         <v>157</v>
       </c>
@@ -29617,7 +29649,7 @@
       <c r="A23" s="208">
         <v>16</v>
       </c>
-      <c r="B23" s="661"/>
+      <c r="B23" s="662"/>
       <c r="C23" s="227" t="s">
         <v>158</v>
       </c>
@@ -29648,7 +29680,7 @@
       <c r="A24" s="208">
         <v>17</v>
       </c>
-      <c r="B24" s="661"/>
+      <c r="B24" s="662"/>
       <c r="C24" s="227" t="s">
         <v>159</v>
       </c>
@@ -29679,7 +29711,7 @@
       <c r="A25" s="208">
         <v>18</v>
       </c>
-      <c r="B25" s="661"/>
+      <c r="B25" s="662"/>
       <c r="C25" s="227" t="s">
         <v>160</v>
       </c>
@@ -29710,7 +29742,7 @@
       <c r="A26" s="208">
         <v>19</v>
       </c>
-      <c r="B26" s="661"/>
+      <c r="B26" s="662"/>
       <c r="C26" s="227" t="s">
         <v>161</v>
       </c>
@@ -29741,7 +29773,7 @@
       <c r="A27" s="214">
         <v>20</v>
       </c>
-      <c r="B27" s="662"/>
+      <c r="B27" s="663"/>
       <c r="C27" s="257" t="s">
         <v>162</v>
       </c>
@@ -29772,7 +29804,7 @@
       <c r="A28" s="204">
         <v>21</v>
       </c>
-      <c r="B28" s="656" t="s">
+      <c r="B28" s="657" t="s">
         <v>323</v>
       </c>
       <c r="C28" s="221" t="s">
@@ -29805,7 +29837,7 @@
       <c r="A29" s="208">
         <v>22</v>
       </c>
-      <c r="B29" s="657"/>
+      <c r="B29" s="658"/>
       <c r="C29" s="224" t="s">
         <v>154</v>
       </c>
@@ -29836,7 +29868,7 @@
       <c r="A30" s="208">
         <v>23</v>
       </c>
-      <c r="B30" s="657"/>
+      <c r="B30" s="658"/>
       <c r="C30" s="227" t="s">
         <v>155</v>
       </c>
@@ -29867,7 +29899,7 @@
       <c r="A31" s="208">
         <v>24</v>
       </c>
-      <c r="B31" s="657"/>
+      <c r="B31" s="658"/>
       <c r="C31" s="227" t="s">
         <v>156</v>
       </c>
@@ -29898,7 +29930,7 @@
       <c r="A32" s="208">
         <v>25</v>
       </c>
-      <c r="B32" s="657"/>
+      <c r="B32" s="658"/>
       <c r="C32" s="227" t="s">
         <v>157</v>
       </c>
@@ -29929,7 +29961,7 @@
       <c r="A33" s="208">
         <v>26</v>
       </c>
-      <c r="B33" s="657"/>
+      <c r="B33" s="658"/>
       <c r="C33" s="227" t="s">
         <v>158</v>
       </c>
@@ -29960,7 +29992,7 @@
       <c r="A34" s="208">
         <v>27</v>
       </c>
-      <c r="B34" s="657"/>
+      <c r="B34" s="658"/>
       <c r="C34" s="227" t="s">
         <v>159</v>
       </c>
@@ -29991,7 +30023,7 @@
       <c r="A35" s="208">
         <v>28</v>
       </c>
-      <c r="B35" s="657"/>
+      <c r="B35" s="658"/>
       <c r="C35" s="227" t="s">
         <v>160</v>
       </c>
@@ -30022,7 +30054,7 @@
       <c r="A36" s="214">
         <v>29</v>
       </c>
-      <c r="B36" s="658"/>
+      <c r="B36" s="659"/>
       <c r="C36" s="257" t="s">
         <v>161</v>
       </c>
@@ -30053,7 +30085,7 @@
       <c r="A37" s="437">
         <v>30</v>
       </c>
-      <c r="B37" s="657" t="s">
+      <c r="B37" s="658" t="s">
         <v>324</v>
       </c>
       <c r="C37" s="237" t="s">
@@ -30086,7 +30118,7 @@
       <c r="A38" s="208">
         <v>31</v>
       </c>
-      <c r="B38" s="657"/>
+      <c r="B38" s="658"/>
       <c r="C38" s="224" t="s">
         <v>154</v>
       </c>
@@ -30117,7 +30149,7 @@
       <c r="A39" s="208">
         <v>32</v>
       </c>
-      <c r="B39" s="657"/>
+      <c r="B39" s="658"/>
       <c r="C39" s="227" t="s">
         <v>155</v>
       </c>
@@ -30148,7 +30180,7 @@
       <c r="A40" s="208">
         <v>33</v>
       </c>
-      <c r="B40" s="657"/>
+      <c r="B40" s="658"/>
       <c r="C40" s="227" t="s">
         <v>156</v>
       </c>
@@ -30179,7 +30211,7 @@
       <c r="A41" s="208">
         <v>34</v>
       </c>
-      <c r="B41" s="657"/>
+      <c r="B41" s="658"/>
       <c r="C41" s="227" t="s">
         <v>157</v>
       </c>
@@ -30210,7 +30242,7 @@
       <c r="A42" s="208">
         <v>35</v>
       </c>
-      <c r="B42" s="657"/>
+      <c r="B42" s="658"/>
       <c r="C42" s="227" t="s">
         <v>158</v>
       </c>
@@ -30241,7 +30273,7 @@
       <c r="A43" s="208">
         <v>36</v>
       </c>
-      <c r="B43" s="657"/>
+      <c r="B43" s="658"/>
       <c r="C43" s="227" t="s">
         <v>159</v>
       </c>
@@ -30272,7 +30304,7 @@
       <c r="A44" s="208">
         <v>37</v>
       </c>
-      <c r="B44" s="657"/>
+      <c r="B44" s="658"/>
       <c r="C44" s="227" t="s">
         <v>160</v>
       </c>
@@ -30303,7 +30335,7 @@
       <c r="A45" s="208">
         <v>38</v>
       </c>
-      <c r="B45" s="657"/>
+      <c r="B45" s="658"/>
       <c r="C45" s="227" t="s">
         <v>161</v>
       </c>
@@ -30334,7 +30366,7 @@
       <c r="A46" s="204">
         <v>39</v>
       </c>
-      <c r="B46" s="656" t="s">
+      <c r="B46" s="657" t="s">
         <v>369</v>
       </c>
       <c r="C46" s="221" t="s">
@@ -30359,7 +30391,7 @@
       <c r="A47" s="208">
         <v>40</v>
       </c>
-      <c r="B47" s="657"/>
+      <c r="B47" s="658"/>
       <c r="C47" s="227" t="s">
         <v>154</v>
       </c>
@@ -30382,7 +30414,7 @@
       <c r="A48" s="208">
         <v>41</v>
       </c>
-      <c r="B48" s="657"/>
+      <c r="B48" s="658"/>
       <c r="C48" s="227" t="s">
         <v>155</v>
       </c>
@@ -30405,7 +30437,7 @@
       <c r="A49" s="208">
         <v>42</v>
       </c>
-      <c r="B49" s="657"/>
+      <c r="B49" s="658"/>
       <c r="C49" s="227" t="s">
         <v>156</v>
       </c>
@@ -30428,7 +30460,7 @@
       <c r="A50" s="208">
         <v>43</v>
       </c>
-      <c r="B50" s="657"/>
+      <c r="B50" s="658"/>
       <c r="C50" s="227" t="s">
         <v>157</v>
       </c>
@@ -30451,7 +30483,7 @@
       <c r="A51" s="208">
         <v>44</v>
       </c>
-      <c r="B51" s="657"/>
+      <c r="B51" s="658"/>
       <c r="C51" s="227" t="s">
         <v>158</v>
       </c>
@@ -30474,7 +30506,7 @@
       <c r="A52" s="208">
         <v>45</v>
       </c>
-      <c r="B52" s="657"/>
+      <c r="B52" s="658"/>
       <c r="C52" s="227" t="s">
         <v>159</v>
       </c>
@@ -30497,7 +30529,7 @@
       <c r="A53" s="208">
         <v>46</v>
       </c>
-      <c r="B53" s="657"/>
+      <c r="B53" s="658"/>
       <c r="C53" s="227" t="s">
         <v>160</v>
       </c>
@@ -30520,7 +30552,7 @@
       <c r="A54" s="214">
         <v>47</v>
       </c>
-      <c r="B54" s="658"/>
+      <c r="B54" s="659"/>
       <c r="C54" s="257" t="s">
         <v>161</v>
       </c>
@@ -30543,7 +30575,7 @@
       <c r="A55" s="437">
         <v>48</v>
       </c>
-      <c r="B55" s="656" t="s">
+      <c r="B55" s="657" t="s">
         <v>325</v>
       </c>
       <c r="C55" s="237" t="s">
@@ -30576,7 +30608,7 @@
       <c r="A56" s="208">
         <v>49</v>
       </c>
-      <c r="B56" s="657"/>
+      <c r="B56" s="658"/>
       <c r="C56" s="224" t="s">
         <v>154</v>
       </c>
@@ -30607,7 +30639,7 @@
       <c r="A57" s="208">
         <v>50</v>
       </c>
-      <c r="B57" s="657"/>
+      <c r="B57" s="658"/>
       <c r="C57" s="227" t="s">
         <v>155</v>
       </c>
@@ -30638,7 +30670,7 @@
       <c r="A58" s="208">
         <v>51</v>
       </c>
-      <c r="B58" s="657"/>
+      <c r="B58" s="658"/>
       <c r="C58" s="227" t="s">
         <v>156</v>
       </c>
@@ -30669,7 +30701,7 @@
       <c r="A59" s="208">
         <v>52</v>
       </c>
-      <c r="B59" s="657"/>
+      <c r="B59" s="658"/>
       <c r="C59" s="227" t="s">
         <v>157</v>
       </c>
@@ -30700,7 +30732,7 @@
       <c r="A60" s="208">
         <v>53</v>
       </c>
-      <c r="B60" s="657"/>
+      <c r="B60" s="658"/>
       <c r="C60" s="227" t="s">
         <v>158</v>
       </c>
@@ -30731,7 +30763,7 @@
       <c r="A61" s="208">
         <v>54</v>
       </c>
-      <c r="B61" s="657"/>
+      <c r="B61" s="658"/>
       <c r="C61" s="227" t="s">
         <v>159</v>
       </c>
@@ -30762,7 +30794,7 @@
       <c r="A62" s="208">
         <v>55</v>
       </c>
-      <c r="B62" s="657"/>
+      <c r="B62" s="658"/>
       <c r="C62" s="227" t="s">
         <v>160</v>
       </c>
@@ -30793,7 +30825,7 @@
       <c r="A63" s="214">
         <v>56</v>
       </c>
-      <c r="B63" s="658"/>
+      <c r="B63" s="659"/>
       <c r="C63" s="257" t="s">
         <v>161</v>
       </c>
@@ -30964,17 +30996,17 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A5" s="663" t="s">
+      <c r="A5" s="664" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="666" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="669" t="s">
+      <c r="B5" s="667" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="670" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="670"/>
-      <c r="E5" s="671"/>
+      <c r="D5" s="671"/>
+      <c r="E5" s="672"/>
       <c r="F5" s="515" t="s">
         <v>166</v>
       </c>
@@ -30985,11 +31017,11 @@
       <c r="K5" s="516"/>
     </row>
     <row r="6" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A6" s="664"/>
-      <c r="B6" s="667"/>
-      <c r="C6" s="672"/>
-      <c r="D6" s="673"/>
-      <c r="E6" s="674"/>
+      <c r="A6" s="665"/>
+      <c r="B6" s="668"/>
+      <c r="C6" s="673"/>
+      <c r="D6" s="674"/>
+      <c r="E6" s="675"/>
       <c r="F6" s="517" t="s">
         <v>5</v>
       </c>
@@ -31002,8 +31034,8 @@
       <c r="K6" s="521"/>
     </row>
     <row r="7" spans="1:11" ht="19.899999999999999" customHeight="1">
-      <c r="A7" s="665"/>
-      <c r="B7" s="668"/>
+      <c r="A7" s="666"/>
+      <c r="B7" s="669"/>
       <c r="C7" s="522" t="s">
         <v>73</v>
       </c>
@@ -31601,13 +31633,13 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1">
-      <c r="A5" s="679" t="s">
+      <c r="A5" s="680" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="677" t="s">
+      <c r="B5" s="678" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="575"/>
+      <c r="C5" s="584"/>
       <c r="D5" s="330" t="s">
         <v>168</v>
       </c>
@@ -31615,9 +31647,9 @@
       <c r="F5" s="303"/>
     </row>
     <row r="6" spans="1:6" ht="32.25" customHeight="1">
-      <c r="A6" s="609"/>
-      <c r="B6" s="678"/>
-      <c r="C6" s="576"/>
+      <c r="A6" s="610"/>
+      <c r="B6" s="679"/>
+      <c r="C6" s="585"/>
       <c r="D6" s="123" t="s">
         <v>3</v>
       </c>
@@ -31632,10 +31664,10 @@
       <c r="A7" s="74">
         <v>1</v>
       </c>
-      <c r="B7" s="680" t="s">
+      <c r="B7" s="681" t="s">
         <v>169</v>
       </c>
-      <c r="C7" s="681"/>
+      <c r="C7" s="682"/>
       <c r="D7" s="304">
         <v>1990</v>
       </c>
@@ -31650,10 +31682,10 @@
       <c r="A8" s="75">
         <v>2</v>
       </c>
-      <c r="B8" s="682" t="s">
+      <c r="B8" s="683" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="683"/>
+      <c r="C8" s="684"/>
       <c r="D8" s="306">
         <v>872</v>
       </c>
@@ -31668,7 +31700,7 @@
       <c r="A9" s="75">
         <v>3</v>
       </c>
-      <c r="B9" s="586" t="s">
+      <c r="B9" s="581" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="308" t="s">
@@ -31688,7 +31720,7 @@
       <c r="A10" s="75">
         <v>4</v>
       </c>
-      <c r="B10" s="586"/>
+      <c r="B10" s="581"/>
       <c r="C10" s="308" t="s">
         <v>196</v>
       </c>
@@ -31706,7 +31738,7 @@
       <c r="A11" s="76">
         <v>5</v>
       </c>
-      <c r="B11" s="586"/>
+      <c r="B11" s="581"/>
       <c r="C11" s="311" t="s">
         <v>171</v>
       </c>
@@ -31724,10 +31756,10 @@
       <c r="A12" s="78">
         <v>6</v>
       </c>
-      <c r="B12" s="675" t="s">
+      <c r="B12" s="676" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="676"/>
+      <c r="C12" s="677"/>
       <c r="D12" s="312">
         <v>2265</v>
       </c>
@@ -31806,15 +31838,15 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1">
-      <c r="A5" s="684" t="s">
+      <c r="A5" s="685" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="677" t="s">
+      <c r="B5" s="678" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="686"/>
-      <c r="D5" s="686"/>
-      <c r="E5" s="575"/>
+      <c r="C5" s="687"/>
+      <c r="D5" s="687"/>
+      <c r="E5" s="584"/>
       <c r="F5" s="46" t="s">
         <v>173</v>
       </c>
@@ -31822,11 +31854,11 @@
       <c r="H5" s="301"/>
     </row>
     <row r="6" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A6" s="685"/>
-      <c r="B6" s="678"/>
-      <c r="C6" s="687"/>
-      <c r="D6" s="687"/>
-      <c r="E6" s="576"/>
+      <c r="A6" s="686"/>
+      <c r="B6" s="679"/>
+      <c r="C6" s="688"/>
+      <c r="D6" s="688"/>
+      <c r="E6" s="585"/>
       <c r="F6" s="108" t="s">
         <v>3</v>
       </c>
@@ -31841,12 +31873,12 @@
       <c r="A7" s="74">
         <v>1</v>
       </c>
-      <c r="B7" s="694" t="s">
+      <c r="B7" s="695" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="695"/>
-      <c r="D7" s="695"/>
-      <c r="E7" s="696"/>
+      <c r="C7" s="696"/>
+      <c r="D7" s="696"/>
+      <c r="E7" s="697"/>
       <c r="F7" s="304">
         <v>201</v>
       </c>
@@ -31861,12 +31893,12 @@
       <c r="A8" s="75">
         <v>2</v>
       </c>
-      <c r="B8" s="682" t="s">
+      <c r="B8" s="683" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="697"/>
-      <c r="D8" s="697"/>
-      <c r="E8" s="683"/>
+      <c r="C8" s="698"/>
+      <c r="D8" s="698"/>
+      <c r="E8" s="684"/>
       <c r="F8" s="306">
         <v>865</v>
       </c>
@@ -31881,16 +31913,16 @@
       <c r="A9" s="75">
         <v>3</v>
       </c>
-      <c r="B9" s="691" t="s">
+      <c r="B9" s="692" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="691" t="s">
+      <c r="C9" s="692" t="s">
         <v>119</v>
       </c>
       <c r="D9" s="316" t="s">
         <v>177</v>
       </c>
-      <c r="E9" s="689" t="s">
+      <c r="E9" s="690" t="s">
         <v>178</v>
       </c>
       <c r="F9" s="313">
@@ -31907,12 +31939,12 @@
       <c r="A10" s="75">
         <v>4</v>
       </c>
-      <c r="B10" s="692"/>
-      <c r="C10" s="701"/>
+      <c r="B10" s="693"/>
+      <c r="C10" s="702"/>
       <c r="D10" s="316" t="s">
         <v>179</v>
       </c>
-      <c r="E10" s="690"/>
+      <c r="E10" s="691"/>
       <c r="F10" s="309">
         <v>144</v>
       </c>
@@ -31927,12 +31959,12 @@
       <c r="A11" s="75">
         <v>5</v>
       </c>
-      <c r="B11" s="692"/>
-      <c r="C11" s="694" t="s">
+      <c r="B11" s="693"/>
+      <c r="C11" s="695" t="s">
         <v>120</v>
       </c>
-      <c r="D11" s="699"/>
-      <c r="E11" s="700"/>
+      <c r="D11" s="700"/>
+      <c r="E11" s="701"/>
       <c r="F11" s="309">
         <v>11</v>
       </c>
@@ -31947,12 +31979,12 @@
       <c r="A12" s="75">
         <v>6</v>
       </c>
-      <c r="B12" s="692"/>
-      <c r="C12" s="682" t="s">
+      <c r="B12" s="693"/>
+      <c r="C12" s="683" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="697"/>
-      <c r="E12" s="683"/>
+      <c r="D12" s="698"/>
+      <c r="E12" s="684"/>
       <c r="F12" s="309">
         <v>4</v>
       </c>
@@ -31967,12 +31999,12 @@
       <c r="A13" s="76">
         <v>7</v>
       </c>
-      <c r="B13" s="693"/>
-      <c r="C13" s="698" t="s">
+      <c r="B13" s="694"/>
+      <c r="C13" s="699" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="695"/>
-      <c r="E13" s="696"/>
+      <c r="D13" s="696"/>
+      <c r="E13" s="697"/>
       <c r="F13" s="309">
         <v>9</v>
       </c>
@@ -31987,12 +32019,12 @@
       <c r="A14" s="78">
         <v>8</v>
       </c>
-      <c r="B14" s="675" t="s">
+      <c r="B14" s="676" t="s">
         <v>182</v>
       </c>
-      <c r="C14" s="688"/>
-      <c r="D14" s="688"/>
-      <c r="E14" s="676"/>
+      <c r="C14" s="689"/>
+      <c r="D14" s="689"/>
+      <c r="E14" s="677"/>
       <c r="F14" s="312">
         <v>202</v>
       </c>
@@ -33705,44 +33737,44 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="23.25" customHeight="1">
-      <c r="A6" s="579" t="s">
+      <c r="A6" s="586" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="577" t="s">
+      <c r="B6" s="576" t="s">
         <v>280</v>
       </c>
-      <c r="C6" s="575" t="s">
+      <c r="C6" s="584" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="577" t="s">
+      <c r="D6" s="576" t="s">
         <v>275</v>
       </c>
-      <c r="E6" s="581" t="s">
+      <c r="E6" s="574" t="s">
         <v>270</v>
       </c>
-      <c r="F6" s="582"/>
-      <c r="G6" s="577" t="s">
+      <c r="F6" s="575"/>
+      <c r="G6" s="576" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="42" customHeight="1">
-      <c r="A7" s="580"/>
-      <c r="B7" s="578"/>
-      <c r="C7" s="576"/>
-      <c r="D7" s="574"/>
+      <c r="A7" s="587"/>
+      <c r="B7" s="582"/>
+      <c r="C7" s="585"/>
+      <c r="D7" s="577"/>
       <c r="E7" s="333" t="s">
         <v>277</v>
       </c>
       <c r="F7" s="334" t="s">
         <v>278</v>
       </c>
-      <c r="G7" s="574"/>
+      <c r="G7" s="577"/>
     </row>
     <row r="8" spans="1:7" ht="30" customHeight="1">
       <c r="A8" s="347">
         <v>1</v>
       </c>
-      <c r="B8" s="583" t="s">
+      <c r="B8" s="578" t="s">
         <v>224</v>
       </c>
       <c r="C8" s="348">
@@ -33765,7 +33797,7 @@
       <c r="A9" s="335">
         <v>2</v>
       </c>
-      <c r="B9" s="584"/>
+      <c r="B9" s="579"/>
       <c r="C9" s="345">
         <f>C8+1</f>
         <v>2016</v>
@@ -33787,7 +33819,7 @@
       <c r="A10" s="335">
         <v>3</v>
       </c>
-      <c r="B10" s="584"/>
+      <c r="B10" s="579"/>
       <c r="C10" s="344">
         <f>C8+2</f>
         <v>2017</v>
@@ -33809,7 +33841,7 @@
       <c r="A11" s="335">
         <v>4</v>
       </c>
-      <c r="B11" s="584"/>
+      <c r="B11" s="579"/>
       <c r="C11" s="344">
         <f>C8+3</f>
         <v>2018</v>
@@ -33831,7 +33863,7 @@
       <c r="A12" s="335">
         <v>5</v>
       </c>
-      <c r="B12" s="584"/>
+      <c r="B12" s="579"/>
       <c r="C12" s="346">
         <f>C8+4</f>
         <v>2019</v>
@@ -33853,7 +33885,7 @@
       <c r="A13" s="339">
         <v>6</v>
       </c>
-      <c r="B13" s="585"/>
+      <c r="B13" s="580"/>
       <c r="C13" s="351">
         <f>C8+5</f>
         <v>2020</v>
@@ -33875,7 +33907,7 @@
       <c r="A14" s="335">
         <v>7</v>
       </c>
-      <c r="B14" s="586" t="s">
+      <c r="B14" s="581" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="344">
@@ -33899,7 +33931,7 @@
       <c r="A15" s="335">
         <v>8</v>
       </c>
-      <c r="B15" s="586"/>
+      <c r="B15" s="581"/>
       <c r="C15" s="345">
         <f>C8+1</f>
         <v>2016</v>
@@ -33921,7 +33953,7 @@
       <c r="A16" s="335">
         <v>9</v>
       </c>
-      <c r="B16" s="586"/>
+      <c r="B16" s="581"/>
       <c r="C16" s="344">
         <f>C8+2</f>
         <v>2017</v>
@@ -33943,7 +33975,7 @@
       <c r="A17" s="335">
         <v>10</v>
       </c>
-      <c r="B17" s="586"/>
+      <c r="B17" s="581"/>
       <c r="C17" s="344">
         <f>C8+3</f>
         <v>2018</v>
@@ -33965,7 +33997,7 @@
       <c r="A18" s="335">
         <v>11</v>
       </c>
-      <c r="B18" s="586"/>
+      <c r="B18" s="581"/>
       <c r="C18" s="346">
         <f>C8+4</f>
         <v>2019</v>
@@ -33987,7 +34019,7 @@
       <c r="A19" s="339">
         <v>12</v>
       </c>
-      <c r="B19" s="578"/>
+      <c r="B19" s="582"/>
       <c r="C19" s="106">
         <f>C8+5</f>
         <v>2020</v>
@@ -34009,7 +34041,7 @@
       <c r="A20" s="335">
         <v>13</v>
       </c>
-      <c r="B20" s="573" t="s">
+      <c r="B20" s="583" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="344">
@@ -34033,7 +34065,7 @@
       <c r="A21" s="335">
         <v>14</v>
       </c>
-      <c r="B21" s="573"/>
+      <c r="B21" s="583"/>
       <c r="C21" s="345">
         <f>C8+1</f>
         <v>2016</v>
@@ -34055,7 +34087,7 @@
       <c r="A22" s="335">
         <v>15</v>
       </c>
-      <c r="B22" s="573"/>
+      <c r="B22" s="583"/>
       <c r="C22" s="344">
         <f>C8+2</f>
         <v>2017</v>
@@ -34077,7 +34109,7 @@
       <c r="A23" s="335">
         <v>16</v>
       </c>
-      <c r="B23" s="573"/>
+      <c r="B23" s="583"/>
       <c r="C23" s="344">
         <f>C8+3</f>
         <v>2018</v>
@@ -34099,7 +34131,7 @@
       <c r="A24" s="335">
         <v>17</v>
       </c>
-      <c r="B24" s="573"/>
+      <c r="B24" s="583"/>
       <c r="C24" s="346">
         <f>C8+4</f>
         <v>2019</v>
@@ -34121,7 +34153,7 @@
       <c r="A25" s="339">
         <v>18</v>
       </c>
-      <c r="B25" s="574"/>
+      <c r="B25" s="577"/>
       <c r="C25" s="14">
         <f>C8+5</f>
         <v>2020</v>
@@ -34155,6 +34187,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="B8:B13"/>
@@ -34162,8 +34196,6 @@
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.70866141732283472" bottom="0.59055118110236227" header="0.43307086614173229" footer="0.51181102362204722"/>

</xml_diff>